<commit_message>
Agregado de archivos de firmware completos en carpeta Firmware.
</commit_message>
<xml_diff>
--- a/Documentación/Lista de Materiales.xlsx
+++ b/Documentación/Lista de Materiales.xlsx
@@ -15,14 +15,14 @@
     <sheet name="PonchoERG" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">PonchoERG!$A$1:$E$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">PonchoERG!$A$1:$E$112</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="191">
   <si>
     <t>Reference</t>
   </si>
@@ -261,6 +261,9 @@
     <t>0.1uF</t>
   </si>
   <si>
+    <t>399-1170-1-ND</t>
+  </si>
+  <si>
     <t>C20</t>
   </si>
   <si>
@@ -270,12 +273,18 @@
     <t>http://www.kemet.com/Lists/ProductCatalog/Attachments/19/KEM_C1006_X5R_SMD.pdf</t>
   </si>
   <si>
+    <t>399-8012-1-ND</t>
+  </si>
+  <si>
     <t>C21</t>
   </si>
   <si>
     <t>1uF</t>
   </si>
   <si>
+    <t>399-1284-1-ND</t>
+  </si>
+  <si>
     <t>C23</t>
   </si>
   <si>
@@ -288,6 +297,9 @@
     <t>Capacitors_SMD:C_1206</t>
   </si>
   <si>
+    <t>399-11631-1-ND</t>
+  </si>
+  <si>
     <t>C24</t>
   </si>
   <si>
@@ -306,112 +318,127 @@
     <t>C29</t>
   </si>
   <si>
+    <t>R19</t>
+  </si>
+  <si>
+    <t>311-0.0ARCT-ND</t>
+  </si>
+  <si>
+    <t>R20</t>
+  </si>
+  <si>
+    <t>390k</t>
+  </si>
+  <si>
+    <t>311-390KARCT-ND</t>
+  </si>
+  <si>
+    <t>C35</t>
+  </si>
+  <si>
+    <t>0.01uF</t>
+  </si>
+  <si>
+    <t>399-1158-1-ND</t>
+  </si>
+  <si>
+    <t>JP2</t>
+  </si>
+  <si>
+    <t>JUMPER</t>
+  </si>
+  <si>
+    <t>Pin_Headers:Pin_Header_Straight_1x02</t>
+  </si>
+  <si>
+    <t>JP1</t>
+  </si>
+  <si>
+    <t>JUMPER3</t>
+  </si>
+  <si>
+    <t>Pin_Headers:Pin_Header_Straight_1x03</t>
+  </si>
+  <si>
+    <t>U14</t>
+  </si>
+  <si>
+    <t>OPA2376</t>
+  </si>
+  <si>
+    <t>SMD_Packages:SOIC-8-N</t>
+  </si>
+  <si>
+    <t>http://www.ti.com/lit/ds/symlink/opa2376.pdf</t>
+  </si>
+  <si>
+    <t>296-22564-1-ND</t>
+  </si>
+  <si>
+    <t>R21</t>
+  </si>
+  <si>
+    <t>10k</t>
+  </si>
+  <si>
+    <t>311-10KARCT-ND</t>
+  </si>
+  <si>
+    <t>C36</t>
+  </si>
+  <si>
+    <t>C37</t>
+  </si>
+  <si>
+    <t>JP3</t>
+  </si>
+  <si>
+    <t>R23</t>
+  </si>
+  <si>
+    <t>R22</t>
+  </si>
+  <si>
+    <t>C38</t>
+  </si>
+  <si>
+    <t>R24</t>
+  </si>
+  <si>
+    <t>JP4</t>
+  </si>
+  <si>
+    <t>C39</t>
+  </si>
+  <si>
+    <t>C40</t>
+  </si>
+  <si>
     <t>J2</t>
   </si>
   <si>
-    <t>I/O's Multi PropÃ³sito</t>
-  </si>
-  <si>
-    <t>Pin_Headers:Pin_Header_Straight_1x04</t>
-  </si>
-  <si>
-    <t>R19</t>
-  </si>
-  <si>
-    <t>311-0.0ARCT-ND</t>
-  </si>
-  <si>
-    <t>R20</t>
-  </si>
-  <si>
-    <t>390k</t>
-  </si>
-  <si>
-    <t>311-390KARCT-ND</t>
-  </si>
-  <si>
-    <t>C35</t>
-  </si>
-  <si>
-    <t>0.01uF</t>
-  </si>
-  <si>
-    <t>JP2</t>
-  </si>
-  <si>
-    <t>JUMPER</t>
-  </si>
-  <si>
-    <t>Pin_Headers:Pin_Header_Straight_1x02</t>
-  </si>
-  <si>
-    <t>JP1</t>
-  </si>
-  <si>
-    <t>JUMPER3</t>
-  </si>
-  <si>
-    <t>Pin_Headers:Pin_Header_Straight_1x03</t>
-  </si>
-  <si>
-    <t>U14</t>
-  </si>
-  <si>
-    <t>OPA2376</t>
-  </si>
-  <si>
-    <t>SMD_Packages:SOIC-8-N</t>
-  </si>
-  <si>
-    <t>http://www.ti.com/lit/ds/symlink/opa2376.pdf</t>
-  </si>
-  <si>
-    <t>296-22564-1-ND</t>
-  </si>
-  <si>
-    <t>R21</t>
-  </si>
-  <si>
-    <t>10k</t>
-  </si>
-  <si>
-    <t>311-10KARCT-ND</t>
-  </si>
-  <si>
-    <t>C36</t>
-  </si>
-  <si>
-    <t>C37</t>
-  </si>
-  <si>
-    <t>JP3</t>
-  </si>
-  <si>
-    <t>R23</t>
-  </si>
-  <si>
-    <t>R22</t>
-  </si>
-  <si>
-    <t>C38</t>
-  </si>
-  <si>
-    <t>R24</t>
-  </si>
-  <si>
-    <t>JP4</t>
-  </si>
-  <si>
-    <t>C39</t>
-  </si>
-  <si>
-    <t>C40</t>
-  </si>
-  <si>
-    <t>JP5</t>
-  </si>
-  <si>
-    <t>AVSS(-)</t>
+    <t>IOs MultipropÃ³sito</t>
+  </si>
+  <si>
+    <t>Pin_Headers:Pin_Header_Straight_1x05</t>
+  </si>
+  <si>
+    <t>Jumper_STD1</t>
+  </si>
+  <si>
+    <t>J_STD</t>
+  </si>
+  <si>
+    <t>footprints:Jumpers_Default</t>
+  </si>
+  <si>
+    <t>NONE</t>
+  </si>
+  <si>
+    <t>Jumper_Config1</t>
+  </si>
+  <si>
+    <t>J_CFG</t>
   </si>
   <si>
     <t>U13</t>
@@ -477,7 +504,10 @@
     <t>Poncho_Esqueleto:Conn_Poncho_Izquierdo</t>
   </si>
   <si>
-    <t>S7123-ND</t>
+    <t>https://media.digikey.com/PDF/Data%20Sheets/Sullins%20PDFs/xRxCzzzDxxN-RC_11636-B.pdf</t>
+  </si>
+  <si>
+    <t>S2011EC-20-ND</t>
   </si>
   <si>
     <t>L2</t>
@@ -495,14 +525,83 @@
     <t>L1</t>
   </si>
   <si>
-    <t>http://www.sullinscorp.com/drawings/78_P(N)PxCxxxLFBN-RC_10492-H.pdf</t>
+    <t>C43</t>
+  </si>
+  <si>
+    <t>C44</t>
+  </si>
+  <si>
+    <t>C45</t>
+  </si>
+  <si>
+    <t>FD1</t>
+  </si>
+  <si>
+    <t>Fiducial</t>
+  </si>
+  <si>
+    <t>Fiducials:Fiducial_1mm_Dia_2.54mm_Outer_CopperTop</t>
+  </si>
+  <si>
+    <t>FD2</t>
+  </si>
+  <si>
+    <t>FD3</t>
+  </si>
+  <si>
+    <t>FD4</t>
+  </si>
+  <si>
+    <t>MH2</t>
+  </si>
+  <si>
+    <t>PCB_HOLE</t>
+  </si>
+  <si>
+    <t>Connect:1pin</t>
+  </si>
+  <si>
+    <t>MH3</t>
+  </si>
+  <si>
+    <t>MH4</t>
+  </si>
+  <si>
+    <t>MH1</t>
+  </si>
+  <si>
+    <t>FD9</t>
+  </si>
+  <si>
+    <t>FD5</t>
+  </si>
+  <si>
+    <t>FD6</t>
+  </si>
+  <si>
+    <t>FD7</t>
+  </si>
+  <si>
+    <t>FD8</t>
+  </si>
+  <si>
+    <t>SC_2</t>
+  </si>
+  <si>
+    <t>Slot_2</t>
+  </si>
+  <si>
+    <t>SC_1</t>
+  </si>
+  <si>
+    <t>Slot_1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -633,14 +732,6 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -943,7 +1034,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="43">
+  <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -986,16 +1077,14 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
   </cellXfs>
-  <cellStyles count="43">
+  <cellStyles count="42">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Énfasis2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Énfasis3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -1027,7 +1116,6 @@
     <cellStyle name="Énfasis5" xfId="34" builtinId="45" customBuiltin="1"/>
     <cellStyle name="Énfasis6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="Entrada" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Hipervínculo" xfId="42" builtinId="8"/>
     <cellStyle name="Incorrecto" xfId="7" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1316,1505 +1404,1914 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E93"/>
+  <dimension ref="A1:E112"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A84" sqref="A84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="40.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" customWidth="1"/>
+    <col min="2" max="2" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="47.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="95.77734375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="25.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="C6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="A7" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" t="s">
-        <v>16</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="C7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="A8" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8" t="s">
+      <c r="C8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="A9" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E9" t="s">
+      <c r="C9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="A10" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C10" t="s">
-        <v>15</v>
-      </c>
-      <c r="D10" t="s">
-        <v>16</v>
-      </c>
-      <c r="E10" t="s">
+      <c r="C10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="A11" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C11" t="s">
-        <v>15</v>
-      </c>
-      <c r="D11" t="s">
-        <v>16</v>
-      </c>
-      <c r="E11" t="s">
+      <c r="C11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="A12" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C12" t="s">
-        <v>15</v>
-      </c>
-      <c r="D12" t="s">
-        <v>16</v>
-      </c>
-      <c r="E12" t="s">
+      <c r="C12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="A13" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C13" t="s">
-        <v>15</v>
-      </c>
-      <c r="D13" t="s">
-        <v>16</v>
-      </c>
-      <c r="E13" t="s">
+      <c r="C13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="A14" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C14" t="s">
-        <v>15</v>
-      </c>
-      <c r="D14" t="s">
-        <v>16</v>
-      </c>
-      <c r="E14" t="s">
+      <c r="C14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+      <c r="A15" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C15" t="s">
-        <v>15</v>
-      </c>
-      <c r="D15" t="s">
-        <v>16</v>
-      </c>
-      <c r="E15" t="s">
+      <c r="C15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+      <c r="A16" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C16" t="s">
-        <v>15</v>
-      </c>
-      <c r="D16" t="s">
-        <v>16</v>
-      </c>
-      <c r="E16" t="s">
+      <c r="C16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+      <c r="A17" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C17" t="s">
-        <v>15</v>
-      </c>
-      <c r="D17" t="s">
-        <v>16</v>
-      </c>
-      <c r="E17" t="s">
+      <c r="C17" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E17" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+      <c r="A18" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C18" t="s">
-        <v>15</v>
-      </c>
-      <c r="D18" t="s">
-        <v>16</v>
-      </c>
-      <c r="E18" t="s">
+      <c r="C18" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+      <c r="A19" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C19" t="s">
-        <v>15</v>
-      </c>
-      <c r="D19" t="s">
-        <v>16</v>
-      </c>
-      <c r="E19" t="s">
+      <c r="C19" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+      <c r="A20" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C20" t="s">
-        <v>15</v>
-      </c>
-      <c r="D20" t="s">
-        <v>16</v>
-      </c>
-      <c r="E20" t="s">
+      <c r="C20" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E20" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+      <c r="A21" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C21" t="s">
-        <v>15</v>
-      </c>
-      <c r="D21" t="s">
-        <v>16</v>
-      </c>
-      <c r="E21" t="s">
+      <c r="C21" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E21" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+      <c r="A22" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E22" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+      <c r="A23" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E23" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+      <c r="A24" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E24" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+      <c r="A25" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E25" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+      <c r="A26" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E26" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
+      <c r="A27" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D27" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E27" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
+      <c r="A28" s="1" t="s">
         <v>39</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C28" t="s">
-        <v>15</v>
-      </c>
-      <c r="D28" t="s">
-        <v>16</v>
-      </c>
-      <c r="E28" t="s">
+      <c r="C28" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E28" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
+      <c r="A29" s="1" t="s">
         <v>40</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C29" t="s">
-        <v>15</v>
-      </c>
-      <c r="D29" t="s">
-        <v>16</v>
-      </c>
-      <c r="E29" t="s">
+      <c r="C29" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E29" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
+      <c r="A30" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D30" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E30" s="1" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
+      <c r="A31" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D31" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E31" s="1" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
+      <c r="A32" s="1" t="s">
         <v>47</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D32" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E32" s="1" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
+      <c r="A33" s="1" t="s">
         <v>48</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D33" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E33" t="s">
+      <c r="E33" s="1" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
+      <c r="A34" s="1" t="s">
         <v>49</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D34" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E34" t="s">
+      <c r="E34" s="1" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
+      <c r="A35" s="1" t="s">
         <v>50</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C35" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D35" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E35" t="s">
+      <c r="E35" s="1" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
+      <c r="A36" s="1" t="s">
         <v>51</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C36" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D36" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E36" t="s">
+      <c r="E36" s="1" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
+      <c r="A37" s="1" t="s">
         <v>52</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C37" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D37" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E37" t="s">
+      <c r="E37" s="1" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
+      <c r="A38" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C38" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D38" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E38" t="s">
+      <c r="E38" s="1" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
+      <c r="A39" s="1" t="s">
         <v>54</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C39" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D39" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E39" t="s">
+      <c r="E39" s="1" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
+      <c r="A40" s="1" t="s">
         <v>55</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C40" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D40" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E40" t="s">
+      <c r="E40" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
+      <c r="A41" s="1" t="s">
         <v>56</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C41" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D41" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E41" t="s">
+      <c r="E41" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
+      <c r="A42" s="1" t="s">
         <v>57</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C42" t="s">
-        <v>15</v>
-      </c>
-      <c r="D42" t="s">
-        <v>16</v>
-      </c>
-      <c r="E42" t="s">
+      <c r="C42" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E42" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
+      <c r="A43" s="1" t="s">
         <v>58</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C43" t="s">
-        <v>15</v>
-      </c>
-      <c r="D43" t="s">
-        <v>16</v>
-      </c>
-      <c r="E43" t="s">
+      <c r="C43" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E43" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
+      <c r="A44" s="1" t="s">
         <v>59</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C44" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D44" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="E44" t="s">
+      <c r="E44" s="1" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
+      <c r="A45" s="1" t="s">
         <v>64</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C45" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D45" t="s">
+      <c r="D45" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E45" t="s">
+      <c r="E45" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
+      <c r="A46" s="1" t="s">
         <v>65</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C46" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D46" t="s">
+      <c r="D46" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E46" t="s">
+      <c r="E46" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
+      <c r="A47" s="1" t="s">
         <v>66</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C47" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D47" t="s">
+      <c r="D47" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E47" t="s">
+      <c r="E47" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
+      <c r="A48" s="1" t="s">
         <v>67</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C48" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D48" t="s">
+      <c r="D48" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E48" t="s">
+      <c r="E48" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
+      <c r="A49" s="1" t="s">
         <v>68</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C49" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D49" t="s">
+      <c r="D49" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E49" t="s">
+      <c r="E49" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
+      <c r="A50" s="1" t="s">
         <v>69</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C50" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D50" t="s">
+      <c r="D50" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E50" t="s">
+      <c r="E50" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
+      <c r="A51" s="1" t="s">
         <v>70</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C51" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D51" t="s">
+      <c r="D51" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E51" t="s">
+      <c r="E51" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
+      <c r="A52" s="1" t="s">
         <v>71</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C52" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D52" t="s">
+      <c r="D52" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="E52" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
+      <c r="A53" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C53" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="D53" t="s">
+      <c r="D53" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="E53" t="s">
+      <c r="E53" s="1" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
+      <c r="A54" s="1" t="s">
         <v>77</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C54" t="s">
-        <v>15</v>
-      </c>
-      <c r="D54" t="s">
-        <v>16</v>
+      <c r="C54" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
-        <v>79</v>
+      <c r="A55" s="1" t="s">
+        <v>80</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C55" t="s">
-        <v>15</v>
-      </c>
-      <c r="D55" t="s">
         <v>81</v>
       </c>
+      <c r="C55" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A56" t="s">
+      <c r="A56" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A57" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A58" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D58" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B56" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C56" t="s">
-        <v>15</v>
-      </c>
-      <c r="D56" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A57" t="s">
-        <v>84</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C57" t="s">
-        <v>15</v>
-      </c>
-      <c r="D57" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A58" t="s">
-        <v>85</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C58" t="s">
-        <v>87</v>
-      </c>
-      <c r="D58" t="s">
-        <v>81</v>
+      <c r="E58" s="1" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A59" t="s">
-        <v>88</v>
+      <c r="A59" s="1" t="s">
+        <v>92</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C59" t="s">
-        <v>15</v>
-      </c>
-      <c r="D59" t="s">
-        <v>16</v>
+      <c r="C59" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A60" t="s">
-        <v>89</v>
+      <c r="A60" s="1" t="s">
+        <v>93</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C60" t="s">
-        <v>15</v>
-      </c>
-      <c r="D60" t="s">
-        <v>16</v>
+        <v>85</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A61" t="s">
-        <v>90</v>
+      <c r="A61" s="1" t="s">
+        <v>94</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C61" t="s">
-        <v>15</v>
-      </c>
-      <c r="D61" t="s">
-        <v>16</v>
+      <c r="C61" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A62" t="s">
-        <v>91</v>
+      <c r="A62" s="1" t="s">
+        <v>95</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C62" t="s">
-        <v>15</v>
-      </c>
-      <c r="D62" t="s">
-        <v>16</v>
+        <v>85</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A63" t="s">
-        <v>92</v>
+      <c r="A63" s="1" t="s">
+        <v>96</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C63" t="s">
-        <v>15</v>
-      </c>
-      <c r="D63" t="s">
-        <v>16</v>
+      <c r="C63" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A64" t="s">
-        <v>93</v>
+      <c r="A64" s="1" t="s">
+        <v>97</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C64" t="s">
-        <v>15</v>
-      </c>
-      <c r="D64" t="s">
-        <v>16</v>
+        <v>85</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A65" t="s">
-        <v>94</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="C65" t="s">
-        <v>96</v>
+      <c r="A65" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B65" s="1">
+        <v>0</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A66" t="s">
-        <v>97</v>
-      </c>
-      <c r="B66" s="1">
+      <c r="A66" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A67" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A68" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A69" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A70" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A71" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A72" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A73" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A74" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A75" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B75" s="1">
         <v>0</v>
       </c>
-      <c r="C66" t="s">
+      <c r="C75" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D66" t="s">
+      <c r="D75" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E66" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A67" t="s">
+      <c r="E75" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B67" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="C67" t="s">
-        <v>7</v>
-      </c>
-      <c r="D67" t="s">
-        <v>8</v>
-      </c>
-      <c r="E67" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A68" t="s">
-        <v>102</v>
-      </c>
-      <c r="B68" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="C68" t="s">
-        <v>15</v>
-      </c>
-      <c r="D68" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A69" t="s">
-        <v>104</v>
-      </c>
-      <c r="B69" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="C69" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A70" t="s">
-        <v>107</v>
-      </c>
-      <c r="B70" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="C70" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A71" t="s">
-        <v>110</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="C71" t="s">
-        <v>112</v>
-      </c>
-      <c r="D71" t="s">
-        <v>113</v>
-      </c>
-      <c r="E71" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A72" t="s">
-        <v>115</v>
-      </c>
-      <c r="B72" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="C72" t="s">
-        <v>7</v>
-      </c>
-      <c r="D72" t="s">
-        <v>8</v>
-      </c>
-      <c r="E72" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A73" t="s">
-        <v>118</v>
-      </c>
-      <c r="B73" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C73" t="s">
-        <v>15</v>
-      </c>
-      <c r="D73" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A74" t="s">
-        <v>119</v>
-      </c>
-      <c r="B74" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C74" t="s">
-        <v>15</v>
-      </c>
-      <c r="D74" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A75" t="s">
-        <v>120</v>
-      </c>
-      <c r="B75" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="C75" t="s">
-        <v>109</v>
-      </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A76" t="s">
-        <v>121</v>
+      <c r="A76" s="1" t="s">
+        <v>124</v>
       </c>
       <c r="B76" s="1">
         <v>0</v>
       </c>
-      <c r="C76" t="s">
+      <c r="C76" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D76" t="s">
+      <c r="D76" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E76" t="s">
-        <v>98</v>
+      <c r="E76" s="1" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A77" t="s">
-        <v>122</v>
-      </c>
-      <c r="B77" s="1">
+      <c r="A77" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A78" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B78" s="1">
         <v>0</v>
       </c>
-      <c r="C77" t="s">
+      <c r="C78" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D77" t="s">
+      <c r="D78" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E77" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A78" t="s">
-        <v>123</v>
-      </c>
-      <c r="B78" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C78" t="s">
-        <v>15</v>
-      </c>
-      <c r="D78" t="s">
-        <v>16</v>
+      <c r="E78" s="1" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A79" t="s">
-        <v>124</v>
-      </c>
-      <c r="B79" s="1">
-        <v>0</v>
-      </c>
-      <c r="C79" t="s">
+      <c r="A79" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A80" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E80" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A81" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E81" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A82" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E82" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A83" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E83" s="1"/>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A84" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E84" s="1"/>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A85" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="E85" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A86" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E86" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A87" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E87" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A88" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E88" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A89" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E89" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A90" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="E90" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A91" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="E91" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A92" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="E92" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A93" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C93" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D79" t="s">
-        <v>8</v>
-      </c>
-      <c r="E79" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A80" t="s">
-        <v>125</v>
-      </c>
-      <c r="B80" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="C80" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A81" t="s">
-        <v>126</v>
-      </c>
-      <c r="B81" s="1" t="s">
+      <c r="D93" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="E93" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A94" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D94" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="E94" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A95" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D95" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E95" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A96" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E96" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C81" t="s">
-        <v>15</v>
-      </c>
-      <c r="D81" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A82" t="s">
-        <v>127</v>
-      </c>
-      <c r="B82" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C82" t="s">
-        <v>15</v>
-      </c>
-      <c r="D82" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A83" t="s">
-        <v>128</v>
-      </c>
-      <c r="B83" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="C83" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A84" t="s">
-        <v>130</v>
-      </c>
-      <c r="B84" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="C84" t="s">
-        <v>132</v>
-      </c>
-      <c r="D84" t="s">
-        <v>133</v>
-      </c>
-      <c r="E84" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A85" t="s">
-        <v>135</v>
-      </c>
-      <c r="B85" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C85" t="s">
-        <v>15</v>
-      </c>
-      <c r="D85" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A86" t="s">
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A97" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D97" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E97" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A98" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="D98" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="B86" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C86" t="s">
-        <v>15</v>
-      </c>
-      <c r="D86" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A87" t="s">
-        <v>137</v>
-      </c>
-      <c r="B87" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C87" t="s">
-        <v>15</v>
-      </c>
-      <c r="D87" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A88" t="s">
-        <v>138</v>
-      </c>
-      <c r="B88" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C88" t="s">
-        <v>15</v>
-      </c>
-      <c r="D88" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A89" t="s">
-        <v>139</v>
-      </c>
-      <c r="B89" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="C89" t="s">
-        <v>141</v>
-      </c>
-      <c r="D89" t="s">
-        <v>142</v>
-      </c>
-      <c r="E89" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A90" t="s">
-        <v>144</v>
-      </c>
-      <c r="B90" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="C90" t="s">
-        <v>141</v>
-      </c>
-      <c r="D90" t="s">
-        <v>146</v>
-      </c>
-      <c r="E90" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A91" t="s">
-        <v>148</v>
-      </c>
-      <c r="B91" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="C91" t="s">
-        <v>150</v>
-      </c>
-      <c r="D91" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="E91" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A92" t="s">
-        <v>152</v>
-      </c>
-      <c r="B92" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="C92" t="s">
-        <v>7</v>
-      </c>
-      <c r="D92" t="s">
-        <v>154</v>
-      </c>
-      <c r="E92" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A93" t="s">
-        <v>156</v>
-      </c>
-      <c r="B93" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="C93" t="s">
-        <v>7</v>
-      </c>
-      <c r="D93" t="s">
-        <v>154</v>
-      </c>
-      <c r="E93" t="s">
-        <v>155</v>
-      </c>
+      <c r="E98" s="1"/>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A99" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="D99" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E99" s="1"/>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A100" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="D100" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E100" s="1"/>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A101" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="D101" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E101" s="1"/>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A102" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D102" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E102" s="1"/>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A103" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D103" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E103" s="1"/>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A104" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D104" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E104" s="1"/>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A105" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D105" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E105" s="1"/>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A106" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="D106" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E106" s="1"/>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A107" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="D107" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E107" s="1"/>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A108" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="D108" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E108" s="1"/>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A109" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="D109" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E109" s="1"/>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A110" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="D110" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E110" s="1"/>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A111" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="D111" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E111" s="1"/>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A112" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="D112" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E112" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E1"/>
-  <hyperlinks>
-    <hyperlink ref="D91" r:id="rId1"/>
-  </hyperlinks>
+  <autoFilter ref="A1:E112"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<DocID Value="https://cws.connectedpdf.com/cDocID/0421208B6749D289ADFD9B22F35930F1~6C965382B8B811E6B7477E20B8FA5A5CF4F9CCC8657CA876-7E865C8AE6104B6B-6188D52D0F83FE1ADBBE8600"/>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<VersionID Value="https://cws.connectedpdf.com/cVersionID/0421208B6749D289ADFD9B22F35930F1~6C965383B8B811E6B7477E20B8FA5A5CF4F979B1C3A27DE1-83A3798E9F10FBD1-F033B83BD5A40138E6208600"/>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BEC0B3D0-3EDD-42A1-B4A7-10730A37A19B}">
+  <ds:schemaRefs/>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EC8C13D1-9739-4E17-8336-8492ACF3ACD6}">
+  <ds:schemaRefs/>
+</ds:datastoreItem>
 </file>
</xml_diff>